<commit_message>
Show gameinfos in gameroom
</commit_message>
<xml_diff>
--- a/documents/time-records/Vorlage-0-Zeitaufzeichnung-Sonnerer.xlsx
+++ b/documents/time-records/Vorlage-0-Zeitaufzeichnung-Sonnerer.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sonnerermichael/Desktop/Informatik/4. Semester/PS SoftwareEngineering/Implementierung/g1t1/documents/time-records/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F851AC8-9A8D-C242-A9B7-665DF9CA99BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEDD2599-53FB-B14D-8AC6-D8F5369CC084}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16220" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="59">
   <si>
     <t>Datum</t>
   </si>
@@ -628,7 +628,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="C27" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D56" sqref="D56"/>
+      <selection pane="bottomRight" activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>
@@ -1408,9 +1408,18 @@
       </c>
     </row>
     <row r="56" spans="1:4">
-      <c r="A56" s="8"/>
-      <c r="B56" s="7"/>
-      <c r="D56" s="3"/>
+      <c r="A56" s="8">
+        <v>43978</v>
+      </c>
+      <c r="B56" s="7">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C56" t="s">
+        <v>14</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57" s="8"/>

</xml_diff>